<commit_message>
#UC admin customer : update tracability file because of package changes
</commit_message>
<xml_diff>
--- a/Diagrams/tlacouque-uc-admin-referential-customer/Tableau de tracabilité.xlsx
+++ b/Diagrams/tlacouque-uc-admin-referential-customer/Tableau de tracabilité.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\PDS Repository\crm\Diagrams\tlacouque-uc-admin-referential-customer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="71">
   <si>
     <t>server-rest[api]</t>
   </si>
@@ -152,36 +152,18 @@
     <t>SpringMongoConfig</t>
   </si>
   <si>
-    <t>fr.pds.isintheair.crmtab.tlacouque.uc.admin.ref.customer.dto</t>
-  </si>
-  <si>
-    <t>fr.pds.isintheair.crmtab.tlacouque.uc.admin.ref.customer.model.asynctask</t>
-  </si>
-  <si>
-    <t>fr.pds.isintheair.crmtab.tlacouque.uc.admin.ref.customer.model.entity</t>
-  </si>
-  <si>
-    <t>fr.pds.isintheair.crmtab.tlacouque.uc.admin.ref.customer.model.enumeration</t>
-  </si>
-  <si>
     <t>CustomerType</t>
   </si>
   <si>
     <t>IndependantType</t>
   </si>
   <si>
-    <t>fr.pds.isintheair.crmtab.tlacouque.uc.admin.ref.customer.model.receiver</t>
-  </si>
-  <si>
     <t>NetworkReceiver</t>
   </si>
   <si>
     <t>CheckInternetConnexion</t>
   </si>
   <si>
-    <t>fr.pds.isintheair.crmtab.tlacouque.uc.admin.ref.customer.model.rest</t>
-  </si>
-  <si>
     <t>CustomerService</t>
   </si>
   <si>
@@ -194,21 +176,12 @@
     <t>CRUDCustomerActivity</t>
   </si>
   <si>
-    <t>fr.pds.isintheair.crmtab.tlacouque.uc.admin.ref.customer.view.activity</t>
-  </si>
-  <si>
-    <t>fr.pds.isintheair.crmtab.tlacouque.uc.admin.ref.customer.view.adapter</t>
-  </si>
-  <si>
     <t>CustomerListViewHolder</t>
   </si>
   <si>
     <t>ListCustomerAdapter</t>
   </si>
   <si>
-    <t>fr.pds.isintheair.crmtab.tlacouque.uc.admin.ref.customer.view.fragment</t>
-  </si>
-  <si>
     <t>CreateCustomerAlertDialog</t>
   </si>
   <si>
@@ -233,16 +206,37 @@
     <t>ListCustomerFragment</t>
   </si>
   <si>
-    <t>fr.pds.isintheair.crmtab.tlacouque.uc.admin.ref.customer.view</t>
-  </si>
-  <si>
     <t>MapUtils</t>
   </si>
   <si>
-    <t>fr.pds.isintheair.crmtab.tlacouque.uc.admin.ref.customer</t>
-  </si>
-  <si>
     <t>FormatValidator</t>
+  </si>
+  <si>
+    <t>fr.pds.isintheair.crmtab.controller.broadcastreceiver</t>
+  </si>
+  <si>
+    <t>fr.pds.isintheair.crmtab.controller.adapter</t>
+  </si>
+  <si>
+    <t>fr.pds.isintheair.crmtab.helper</t>
+  </si>
+  <si>
+    <t>fr.pds.isintheair.crmtab.model.asynctask</t>
+  </si>
+  <si>
+    <t>fr.pds.isintheair.crmtab.model.entity</t>
+  </si>
+  <si>
+    <t>fr.pds.isintheair.crmtab.model.rest.service</t>
+  </si>
+  <si>
+    <t>fr.pds.isintheair.crmtab.model.rest</t>
+  </si>
+  <si>
+    <t>fr.pds.isintheair.crmtab.view.activity</t>
+  </si>
+  <si>
+    <t>fr.pds.isintheair.crmtab.view.fragment</t>
   </si>
 </sst>
 </file>
@@ -681,8 +675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +961,7 @@
         <v>5</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>38</v>
@@ -977,7 +971,7 @@
       <c r="B31" s="11"/>
       <c r="C31" s="8"/>
       <c r="D31" s="2" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>39</v>
@@ -987,7 +981,7 @@
       <c r="B32" s="11"/>
       <c r="C32" s="8"/>
       <c r="D32" s="2" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>9</v>
@@ -997,7 +991,7 @@
       <c r="B33" s="11"/>
       <c r="C33" s="8"/>
       <c r="D33" s="2" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>29</v>
@@ -1007,7 +1001,7 @@
       <c r="B34" s="11"/>
       <c r="C34" s="8"/>
       <c r="D34" s="2" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="E34" s="2" t="s">
         <v>35</v>
@@ -1017,7 +1011,7 @@
       <c r="B35" s="11"/>
       <c r="C35" s="8"/>
       <c r="D35" s="2" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>21</v>
@@ -1027,7 +1021,7 @@
       <c r="B36" s="11"/>
       <c r="C36" s="8"/>
       <c r="D36" s="2" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>22</v>
@@ -1037,7 +1031,7 @@
       <c r="B37" s="11"/>
       <c r="C37" s="8"/>
       <c r="D37" s="2" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>30</v>
@@ -1047,7 +1041,7 @@
       <c r="B38" s="11"/>
       <c r="C38" s="8"/>
       <c r="D38" s="2" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>36</v>
@@ -1057,7 +1051,7 @@
       <c r="B39" s="11"/>
       <c r="C39" s="8"/>
       <c r="D39" s="2" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>33</v>
@@ -1067,7 +1061,7 @@
       <c r="B40" s="11"/>
       <c r="C40" s="8"/>
       <c r="D40" s="2" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>23</v>
@@ -1077,7 +1071,7 @@
       <c r="B41" s="11"/>
       <c r="C41" s="8"/>
       <c r="D41" s="2" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="E41" s="2" t="s">
         <v>31</v>
@@ -1087,17 +1081,17 @@
       <c r="B42" s="11"/>
       <c r="C42" s="8"/>
       <c r="D42" s="2" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="11"/>
       <c r="C43" s="8"/>
       <c r="D43" s="2" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>20</v>
@@ -1107,190 +1101,190 @@
       <c r="B44" s="11"/>
       <c r="C44" s="8"/>
       <c r="D44" s="2" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="11"/>
       <c r="C45" s="8"/>
       <c r="D45" s="2" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="11"/>
       <c r="C46" s="8"/>
       <c r="D46" s="2" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="11"/>
       <c r="C47" s="8"/>
       <c r="D47" s="2" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="11"/>
       <c r="C48" s="8"/>
       <c r="D48" s="2" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B49" s="11"/>
       <c r="C49" s="8"/>
       <c r="D49" s="2" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B50" s="11"/>
       <c r="C50" s="8"/>
       <c r="D50" s="2" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B51" s="11"/>
       <c r="C51" s="8"/>
       <c r="D51" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B52" s="11"/>
       <c r="C52" s="8"/>
       <c r="D52" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B53" s="11"/>
       <c r="C53" s="8"/>
       <c r="D53" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B54" s="11"/>
       <c r="C54" s="8"/>
       <c r="D54" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B55" s="11"/>
       <c r="C55" s="8"/>
       <c r="D55" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B56" s="11"/>
       <c r="C56" s="8"/>
       <c r="D56" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B57" s="11"/>
       <c r="C57" s="8"/>
       <c r="D57" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B58" s="11"/>
       <c r="C58" s="8"/>
       <c r="D58" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B59" s="11"/>
       <c r="C59" s="8"/>
       <c r="D59" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B60" s="11"/>
       <c r="C60" s="8"/>
       <c r="D60" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B61" s="11"/>
       <c r="C61" s="8"/>
       <c r="D61" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B62" s="11"/>
       <c r="C62" s="9"/>
       <c r="D62" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>